<commit_message>
research on book the life and times of su tungpo
</commit_message>
<xml_diff>
--- a/readings/书单筛选.xlsx
+++ b/readings/书单筛选.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\github\metathought\readings\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E82E5225-8CE8-4E8D-B50D-299EF3356076}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28695" windowHeight="13065" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="知识树选书" sheetId="1" r:id="rId1"/>
@@ -12,17 +18,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">知识树选书!$A$1:$S$29</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>lqin</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -75,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>领域</t>
   </si>
@@ -392,18 +398,69 @@
 基因组：人体是基因与环境进行交互的一个界面，休谟之叉：我们的行为要么是实现已经被决定的，这样我们不必为它们负责；要么是偶然事件的结果，这样我们也不必为它们负责。
 理性乐观派：交换使得现在是世界成为迄今最好的世界</t>
   </si>
+  <si>
+    <t>传记文学</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>苏东坡传</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>林语堂</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>百花文艺出版社</t>
+  </si>
+  <si>
+    <t>林语堂 1985年-1976年
+中国现代著名作家、学者、翻译家、语言学家。一生翻译大量中国文学，介绍中国文化与风俗。
+将外国幽默一词引入中国，中国“幽默文学”创始人，倡导文章中的“幽默”与“性灵”</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>明清散文，袁宏道、张岱、李渔
+外国幽默文学，萧伯纳
+伊壁鸠鲁的信徒
+基督教家庭，青年又热爱儒学道学
+辜鸿铭</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>梁实秋、沈从文</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>鲁迅，左翼作家联盟</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>“他向西方人士解释他的同胞和国家的风俗，想望，恐惧和思想成就”</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>对外介绍中国精神，风俗人情，对内发扬中英通译，旨在文化交流。因此林的小说皆为英文，而中文作品均为散文，和词典类工具书。主办的杂志以英文译文为主旨。</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>1924 《论士气与思想界之关系》
+1932- 杂志《论语》《人世间》
+《吾国与吾民》，1935
+《孔子的智慧》，1935
+《生活的艺术》，1936 
+《京华烟云》，1935
+《苏东坡传》，1947  作者最偏爱的作品
+《平心论高鹗》，1966
+《林语堂当代汉英词典》，1972</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,13 +479,13 @@
       <sz val="10"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -440,143 +497,32 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <sz val="9"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,7 +531,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79995117038483843"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,182 +541,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -793,255 +565,16 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1057,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="31" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
@@ -1084,59 +617,33 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1392,25 +899,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
-      <selection/>
+      <pane xSplit="2" ySplit="1" topLeftCell="O11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.25" customWidth="1"/>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.875" customWidth="1"/>
     <col min="5" max="5" width="52.5" customWidth="1"/>
     <col min="6" max="6" width="6.75" customWidth="1"/>
@@ -1422,7 +928,7 @@
     <col min="18" max="18" width="6.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="61.5" customHeight="1" spans="1:19">
+    <row r="1" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +987,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="42.75" spans="1:19">
+    <row r="2" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1492,7 +998,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D26" si="0">P2+R2+F2+L2+0.2*S2</f>
+        <f t="shared" ref="D2:D29" si="0">P2+R2+F2+L2+0.2*S2</f>
         <v>21.88</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1529,7 +1035,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="3" ht="114" spans="1:19">
+    <row r="3" spans="1:19" ht="114" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -1584,10 +1090,10 @@
         <v>5</v>
       </c>
       <c r="S3" s="3">
-        <v>8.2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1597,7 +1103,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
-        <v>18.9</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>37</v>
@@ -1633,7 +1139,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" ht="342" spans="1:19">
+    <row r="5" spans="1:19" ht="342" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
@@ -1683,7 +1189,7 @@
         <v>8.4</v>
       </c>
     </row>
-    <row r="6" ht="142.5" spans="1:19">
+    <row r="6" spans="1:19" ht="142.5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
@@ -1738,10 +1244,10 @@
         <v>2</v>
       </c>
       <c r="S6" s="1">
-        <v>8.2</v>
-      </c>
-    </row>
-    <row r="7" ht="42.75" spans="1:19">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -1791,7 +1297,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="8" ht="85.5" spans="1:19">
+    <row r="8" spans="1:19" ht="85.5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>40</v>
       </c>
@@ -1803,7 +1309,7 @@
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
-        <v>16.76</v>
+        <v>16.760000000000002</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>66</v>
@@ -1838,10 +1344,10 @@
         <v>2</v>
       </c>
       <c r="S8" s="1">
-        <v>8.8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -1853,7 +1359,7 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>16.58</v>
+        <v>16.579999999999998</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
@@ -1887,7 +1393,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="10" ht="256.5" spans="1:19">
+    <row r="10" spans="1:19" ht="256.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -1945,139 +1451,186 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="11" spans="4:14">
-      <c r="D11">
-        <f t="shared" ref="D11:D21" si="1">P11+R11+F11+M11+0.2*S11</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="12"/>
-    </row>
-    <row r="12" spans="4:14">
-      <c r="D12">
-        <f t="shared" si="1"/>
+    <row r="11" spans="1:19" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>18.7</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="1">
+        <v>5</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="L11" s="1">
+        <v>5</v>
+      </c>
+      <c r="M11" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="16">
+        <v>2000</v>
+      </c>
+      <c r="R11" s="16">
+        <v>4</v>
+      </c>
+      <c r="S11" s="16">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="4:15">
-      <c r="D13">
-        <f t="shared" si="1"/>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" s="12"/>
       <c r="O13" s="13"/>
     </row>
-    <row r="14" spans="4:14">
-      <c r="D14">
-        <f t="shared" si="1"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="4:14">
-      <c r="D15">
-        <f t="shared" si="1"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="4:14">
-      <c r="D16">
-        <f t="shared" si="1"/>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="4:14">
-      <c r="D17">
-        <f t="shared" si="1"/>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="4:14">
-      <c r="D18">
-        <f t="shared" si="1"/>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="4:14">
-      <c r="D19">
-        <f t="shared" si="1"/>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="4:4">
-      <c r="D20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27">
-        <f t="shared" ref="D27:D29" si="2">P27+R27+F27+L27+0.2*S27</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29">
-        <f t="shared" si="2"/>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.2">
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S29">
-    <sortState ref="A1:S29">
-      <sortCondition ref="D1" descending="1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
+  <autoFilter ref="A1:S29" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update research on 见识
</commit_message>
<xml_diff>
--- a/readings/书单筛选.xlsx
+++ b/readings/书单筛选.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13065"/>
+    <workbookView windowWidth="28080" windowHeight="13065"/>
   </bookViews>
   <sheets>
     <sheet name="知识树选书" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90">
   <si>
     <t>领域</t>
   </si>
@@ -392,6 +392,39 @@
 基因组：人体是基因与环境进行交互的一个界面，休谟之叉：我们的行为要么是实现已经被决定的，这样我们不必为它们负责；要么是偶然事件的结果，这样我们也不必为它们负责。
 理性乐观派：交换使得现在是世界成为迄今最好的世界</t>
   </si>
+  <si>
+    <t>互联网</t>
+  </si>
+  <si>
+    <t>见识</t>
+  </si>
+  <si>
+    <t>吴军</t>
+  </si>
+  <si>
+    <t>吴军
+自然语言处理和搜索专家，硅谷风险投资人。
+吴军博士曾经担任谷歌资深研究员，设计了谷歌中、日、韩文搜索算法以及谷歌的自然语言分析器。2010-2012年担任腾讯负责搜索和搜索广告等业务的副总裁，后回到谷歌负责计算机自动问答项目。
+吴军博士自2008年开始从事风险投资，并于2014年作为创始合伙人创立了硅谷丰元资本风险投资基金。他也是上海交通大学客座研究员和约翰•霍普金斯大学工学院董事。</t>
+  </si>
+  <si>
+    <t>成败与否取决于见识的高低
+优秀的人胜在思维方式</t>
+  </si>
+  <si>
+    <t>《浪潮之巅》，2011 科技公司兴衰史
+《数学之美》，2012 搜索算法的数学基础
+《文明之光》，2014 人类文明观察
+《大学之路》，2015 美国高等教育思考
+《硅谷之谜》，2015 硅谷创业起源
+《智能时代》，2016 机器智能对未来社会的影响
+《见识》，2018 将人生的兴衰归结于认知提升</t>
+  </si>
+  <si>
+    <t>专长、经典《数学之美》
+科技观察，财报解读实例《浪潮之巅》
+元认知《见识》</t>
+  </si>
 </sst>
 </file>
 
@@ -399,8 +432,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -439,6 +472,35 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -447,20 +509,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -468,6 +517,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
@@ -476,7 +572,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,92 +608,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -597,25 +630,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,145 +798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,6 +827,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -805,15 +849,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -833,11 +868,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -861,33 +902,25 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -899,10 +932,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -911,137 +944,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1055,6 +1088,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="31" applyBorder="1">
@@ -1401,11 +1440,11 @@
   <dimension ref="A1:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F10" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1453,7 +1492,7 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
@@ -1513,7 +1552,7 @@
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="8" t="s">
         <v>24</v>
       </c>
       <c r="P2" s="1">
@@ -1571,7 +1610,7 @@
         <v>34</v>
       </c>
       <c r="N3" s="4"/>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="9" t="s">
         <v>35</v>
       </c>
       <c r="P3" s="4">
@@ -1725,7 +1764,7 @@
         <v>56</v>
       </c>
       <c r="N6" s="2"/>
-      <c r="O6" s="8" t="s">
+      <c r="O6" s="10" t="s">
         <v>57</v>
       </c>
       <c r="P6" s="2">
@@ -1774,8 +1813,8 @@
         <v>5</v>
       </c>
       <c r="M7" s="3"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="10" t="s">
+      <c r="N7" s="11"/>
+      <c r="O7" s="12" t="s">
         <v>63</v>
       </c>
       <c r="P7" s="4">
@@ -1825,7 +1864,7 @@
         <v>68</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="8" t="s">
         <v>69</v>
       </c>
       <c r="P8" s="2">
@@ -1871,7 +1910,7 @@
         <v>72</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="P9" s="1">
@@ -1897,8 +1936,8 @@
       <c r="C10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="0"/>
+      <c r="D10" s="5">
+        <f>P10+R10+F10+L10+0.2*S10</f>
         <v>12.54</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -1913,7 +1952,7 @@
       <c r="H10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="2" t="s">
         <v>79</v>
       </c>
       <c r="J10" s="1"/>
@@ -1945,69 +1984,114 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="11" spans="4:14">
-      <c r="D11">
-        <f t="shared" ref="D11:D21" si="1">P11+R11+F11+M11+0.2*S11</f>
-        <v>0</v>
-      </c>
-      <c r="N11" s="12"/>
+    <row r="11" ht="171" spans="1:19">
+      <c r="A11" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="5">
+        <f>P11+R11+F11+L11+0.2*S11</f>
+        <v>15.62</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L11" s="5">
+        <v>5</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P11" s="5">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>2018</v>
+      </c>
+      <c r="R11" s="5">
+        <v>1</v>
+      </c>
+      <c r="S11" s="5">
+        <v>8.1</v>
+      </c>
     </row>
     <row r="12" spans="4:14">
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D11:D21" si="1">P12+R12+F12+M12+0.2*S12</f>
         <v>0</v>
       </c>
-      <c r="N12" s="12"/>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" spans="4:15">
       <c r="D13">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N13" s="12"/>
-      <c r="O13" s="13"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="15"/>
     </row>
     <row r="14" spans="4:14">
       <c r="D14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N14" s="12"/>
+      <c r="N14" s="14"/>
     </row>
     <row r="15" spans="4:14">
       <c r="D15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N15" s="12"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" spans="4:14">
       <c r="D16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N16" s="12"/>
+      <c r="N16" s="14"/>
     </row>
     <row r="17" spans="4:14">
       <c r="D17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N17" s="12"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="4:14">
       <c r="D18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N18" s="12"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="4:14">
       <c r="D19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N19" s="12"/>
+      <c r="N19" s="14"/>
     </row>
     <row r="20" spans="4:4">
       <c r="D20">

</xml_diff>